<commit_message>
Forgot to check in Summer 2019.
</commit_message>
<xml_diff>
--- a/Copy/2019-Summer/WordCount.xlsx
+++ b/Copy/2019-Summer/WordCount.xlsx
@@ -466,7 +466,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -660,10 +660,10 @@
         <v>8</v>
       </c>
       <c r="F9">
-        <v>1888</v>
+        <v>1421</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -683,11 +683,11 @@
       </c>
       <c r="F11">
         <f>SUM(F2:F10)</f>
-        <v>5131</v>
+        <v>4664</v>
       </c>
       <c r="G11">
         <f>SUM(G2:G10)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H11" t="s">
         <v>14</v>
@@ -711,15 +711,15 @@
       </c>
       <c r="F12" s="1">
         <f>F11/600</f>
-        <v>8.5516666666666659</v>
+        <v>7.7733333333333334</v>
       </c>
       <c r="G12" s="1">
         <f>G11/5</f>
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="H12" s="1">
         <f>SUM(F12:G12)</f>
-        <v>12.151666666666666</v>
+        <v>11.173333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>